<commit_message>
feat: add average price search
</commit_message>
<xml_diff>
--- a/ProdutosMercadoLivre.xlsx
+++ b/ProdutosMercadoLivre.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Price</t>
+          <t>AvgPrice</t>
         </is>
       </c>
     </row>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4290</v>
+        <v>4240.1</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8999</v>
+        <v>2315.4</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>48</v>
+        <v>679.4</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>289</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1159</v>
+        <v>1082.4</v>
       </c>
     </row>
     <row r="7">
@@ -502,13 +502,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>349</v>
+        <v>502.4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="n">
-        <v>15134</v>
+        <v>9078.699999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: change class name and file name
</commit_message>
<xml_diff>
--- a/ProdutosMercadoLivre.xlsx
+++ b/ProdutosMercadoLivre.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4240.1</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2315.4</v>
+        <v>2280.1</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>679.4</v>
+        <v>681.5</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>259</v>
+        <v>245.6</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1082.4</v>
+        <v>1115.1</v>
       </c>
     </row>
     <row r="7">
@@ -502,13 +502,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>502.4</v>
+        <v>312.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="n">
-        <v>9078.699999999999</v>
+        <v>8874.400000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>